<commit_message>
Added Gestion du temps
</commit_message>
<xml_diff>
--- a/Dictionnaire de données Fil Rouge.xlsx
+++ b/Dictionnaire de données Fil Rouge.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -743,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1271,6 +1272,9 @@
       <c r="B62" t="s">
         <v>59</v>
       </c>
+      <c r="C62" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -1279,6 +1283,9 @@
       <c r="B63" t="s">
         <v>60</v>
       </c>
+      <c r="C63" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -1287,41 +1294,35 @@
       <c r="B64" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>7</v>
       </c>
       <c r="B65" t="s">
         <v>62</v>
       </c>
-      <c r="C65" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>9</v>
       </c>
       <c r="B66" t="s">
         <v>63</v>
       </c>
-      <c r="C66" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>10</v>
       </c>
       <c r="B67" t="s">
         <v>64</v>
       </c>
-      <c r="C67" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -1329,27 +1330,27 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Added final modifications and begun pptx
</commit_message>
<xml_diff>
--- a/Dictionnaire de données Fil Rouge.xlsx
+++ b/Dictionnaire de données Fil Rouge.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="147">
   <si>
     <t>Entités</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Fichier_Photo</t>
   </si>
   <si>
-    <t>Date_Publi</t>
-  </si>
-  <si>
     <t>Tarif Adhérent</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>RGFAQ02</t>
   </si>
   <si>
-    <t>On peut s'inscrire maxi 5 jours avant la date de début de l'activité</t>
-  </si>
-  <si>
     <t>RG02</t>
   </si>
   <si>
@@ -248,12 +242,6 @@
     <t>RGFAQ07</t>
   </si>
   <si>
-    <t>RGFAQ08</t>
-  </si>
-  <si>
-    <t>RGFAQ09</t>
-  </si>
-  <si>
     <t>email du membre</t>
   </si>
   <si>
@@ -368,9 +356,6 @@
     <t>la date maxi d'inscription à une activité est fixée à la date de l'activité moins 5 jours.</t>
   </si>
   <si>
-    <t>le nombre maximum de participants à une activité est fixé à 50</t>
-  </si>
-  <si>
     <t>C'est une nouvelle pour les adhérents</t>
   </si>
   <si>
@@ -426,13 +411,67 @@
   </si>
   <si>
     <t>Number(5,2)</t>
+  </si>
+  <si>
+    <t>Cotisation à jour</t>
+  </si>
+  <si>
+    <t>Cotisation_A_Jour</t>
+  </si>
+  <si>
+    <t>Date de la cotisation</t>
+  </si>
+  <si>
+    <t>Date_Cotisation</t>
+  </si>
+  <si>
+    <t>Montant de la cotisation</t>
+  </si>
+  <si>
+    <t>Montant_Cotisation</t>
+  </si>
+  <si>
+    <t>Id Saison</t>
+  </si>
+  <si>
+    <t>Id_Saison</t>
+  </si>
+  <si>
+    <t>Date de début de la saison</t>
+  </si>
+  <si>
+    <t>Date_Debut_Saison</t>
+  </si>
+  <si>
+    <t>Date de fin de la saison</t>
+  </si>
+  <si>
+    <t>Date_Fin_Saison</t>
+  </si>
+  <si>
+    <t>Date de la publication</t>
+  </si>
+  <si>
+    <t>Date_Publi_Photo</t>
+  </si>
+  <si>
+    <t>Date_Publi_Nouvelle</t>
+  </si>
+  <si>
+    <t>valeurs calculées</t>
+  </si>
+  <si>
+    <t>nombre de participants à une activité</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +484,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -482,11 +529,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E57" sqref="C3:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,7 +866,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -828,7 +877,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -839,18 +888,18 @@
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -861,18 +910,18 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -880,10 +929,10 @@
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -894,18 +943,18 @@
         <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -916,51 +965,51 @@
         <v>32</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
@@ -976,7 +1025,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
@@ -987,7 +1036,7 @@
         <v>23</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
@@ -998,7 +1047,7 @@
         <v>34</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
@@ -1009,7 +1058,7 @@
         <v>25</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
@@ -1020,7 +1069,7 @@
         <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
@@ -1031,62 +1080,62 @@
         <v>36</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C29" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.3">
@@ -1096,35 +1145,35 @@
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.3">
@@ -1140,7 +1189,7 @@
         <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.3">
@@ -1151,7 +1200,7 @@
         <v>41</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.3">
@@ -1159,10 +1208,10 @@
         <v>39</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.3">
@@ -1172,259 +1221,351 @@
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C43" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C48" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C49" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C50" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C52" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C53" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C54" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C56" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C57" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" t="s">
         <v>112</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
         <v>69</v>
       </c>
-      <c r="C51" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
+      <c r="C64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
         <v>70</v>
       </c>
-      <c r="C52" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
+      <c r="C65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
         <v>71</v>
       </c>
-      <c r="C53" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
-        <v>73</v>
-      </c>
-      <c r="C55" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>74</v>
-      </c>
-      <c r="C56" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" t="s">
-        <v>50</v>
-      </c>
-      <c r="C60" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" t="s">
-        <v>54</v>
-      </c>
-      <c r="C62" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
-        <v>57</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" t="s">
-        <v>58</v>
-      </c>
-      <c r="C65" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" t="s">
-        <v>59</v>
-      </c>
-      <c r="C66" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>7</v>
-      </c>
-      <c r="B67" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>9</v>
-      </c>
-      <c r="B68" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>11</v>
-      </c>
-      <c r="B70" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>64</v>
+        <v>49</v>
+      </c>
+      <c r="C71" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>65</v>
+        <v>46</v>
+      </c>
+      <c r="C72" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>66</v>
+        <v>52</v>
+      </c>
+      <c r="C73" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>67</v>
+        <v>54</v>
+      </c>
+      <c r="C74" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>68</v>
+        <v>55</v>
+      </c>
+      <c r="C75" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>